<commit_message>
đay code ngày 12/04
</commit_message>
<xml_diff>
--- a/bangluudulieu_tamthoi.xlsx
+++ b/bangluudulieu_tamthoi.xlsx
@@ -428,7 +428,7 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -459,18 +459,30 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>43H03154</t>
+          <t>43C22665_C</t>
         </is>
       </c>
     </row>
     <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Tổng số phương tiện be</t>
+        </is>
+      </c>
       <c r="B3" t="n">
-        <v>18</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" t="n">
-        <v>24</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Tổng số phương tiện fe</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
       </c>
     </row>
     <row r="7">

</xml_diff>